<commit_message>
Función "liberar llamado" + Pulida de backend y frontend
</commit_message>
<xml_diff>
--- a/static/usuariosWise.xlsx
+++ b/static/usuariosWise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazaro.gonzalez\Desktop\Widget\api enlaces\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FAD652-A3A5-4D08-9811-C6B6AA90879D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60265A-F8A6-42C0-8416-93498B560235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="86e68854d5064d6ab55e340f957a8b5" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>bruno.filippin@nobis.com.ar</t>
+  </si>
+  <si>
+    <t>Filippin</t>
+  </si>
+  <si>
+    <t>Bruno</t>
   </si>
 </sst>
 </file>
@@ -659,7 +668,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -672,6 +681,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1028,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,7 +1380,27 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>35161</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Melisa - B1 (provisional)
</commit_message>
<xml_diff>
--- a/static/usuariosWise.xlsx
+++ b/static/usuariosWise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazaro.gonzalez\Desktop\Widget\api enlaces\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60265A-F8A6-42C0-8416-93498B560235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6315C-5317-48BE-863D-69C870D88273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="86e68854d5064d6ab55e340f957a8b5" sheetId="1" r:id="rId1"/>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,7 +1170,7 @@
         <v>45803.565879629627</v>
       </c>
       <c r="G5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Cambio Novello - B1
</commit_message>
<xml_diff>
--- a/static/usuariosWise.xlsx
+++ b/static/usuariosWise.xlsx
@@ -181,7 +181,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -564,7 +564,7 @@
     <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>35167</v>
       </c>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>44184</v>
       </c>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>35169</v>
       </c>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>45659</v>
       </c>
@@ -679,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>35163</v>
       </c>
@@ -702,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>36797</v>
       </c>
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>35126</v>
       </c>
@@ -748,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>44175</v>
       </c>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>45599</v>
       </c>
@@ -791,10 +791,10 @@
         <v>45800.950636574074</v>
       </c>
       <c r="G10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>40485</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>38008</v>
       </c>
@@ -840,7 +840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>38356</v>
       </c>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>36798</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="1">
         <v>35161</v>
       </c>

</xml_diff>